<commit_message>
labels: map by PDF order number; grouped outputs + manifest
</commit_message>
<xml_diff>
--- a/data_crm/orders_kaspi_with_sizes.xlsx
+++ b/data_crm/orders_kaspi_with_sizes.xlsx
@@ -476,12 +476,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>my_size</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
           <t>rec_size</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>model_group</t>
         </is>
       </c>
     </row>
@@ -508,7 +508,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>KSP ALMATY-1</t>
+          <t>KSP Almaty-1</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -518,12 +518,12 @@
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>XL</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>MOD123</t>
+          <t>XL</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>KSP ASTANA-2</t>
+          <t>KSP Astana-2</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -565,7 +565,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>MOD456</t>
+          <t>M</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
orders: use shared async http client; graceful Ctrl-C
</commit_message>
<xml_diff>
--- a/data_crm/orders_kaspi_with_sizes.xlsx
+++ b/data_crm/orders_kaspi_with_sizes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,90 +485,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>O-1001</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-08-13</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>KSP-ABC123</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>MOD123</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>KSP Almaty-1</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>XL</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>XL</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>O-1002</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-08-13</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>KSP-XYZ999</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MOD456</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>KSP Astana-2</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>